<commit_message>
my commit of 01-09-2025
</commit_message>
<xml_diff>
--- a/clubs_uniques.xlsx
+++ b/clubs_uniques.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -429,6 +429,576 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CAP/CALT/ST00190</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Centre de Sante Avec Lits Trou-du-Nord</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1991-10-06</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Femmes Vaillantes 6</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Club Mere</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>1- Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CAP/CMBV/ST01939</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CLINIQUE MEDICALE BETHESDA DE VAUDREUIL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1983-07-14</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Synergie</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Club Mere</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>1- Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CAP/HSCM/ST02041</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Hôpital Sacre Coeur de Milot</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2006-09-29</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Fanm vanyan 8</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Club Mere</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>1- Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CAP/SECH/ST00759</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Clinique J-Benjamin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2006-12-24</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>lauriers</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Club Mere</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>1- Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PAP/CMSP/ST00614</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Centre de Santé de Petite Place Cazeau</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1984-09-07</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Safe Place</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Club Mere</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>1- Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>PAP/HBMP/ST03073</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Hôpital Bernard Mevs</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1983-05-08</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Afro-Queen</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Club Mere</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>1- Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PAP/HFSC/ST04390</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Hopital Foyer Saint-Camille</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1998-11-14</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Esperanza</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Club Mere</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>1- Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>PAP/HSFS/ST00157</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>St. Francoise de Sales</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1988-11-07</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Alliance</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Club Mere</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>1- Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>PAP/NPFS/ST00223</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Hôpital Saint Damien NOS PETITS FRERES ET SOEURS (NPFS)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2003-11-08</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Les Roses</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Club Mere</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>1- Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SMA/CSSM/ST00427</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Centre Santé de Saint Michel de l’Attalaye</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1992-01-01</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Ambassadrice 4</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Club Mere</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>1- Present</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>